<commit_message>
pushing the code sent by shaheena.
</commit_message>
<xml_diff>
--- a/src/test/java/com/born/xls/Suite.xlsx
+++ b/src/test/java/com/born/xls/Suite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6795"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14310" windowHeight="3010"/>
   </bookViews>
   <sheets>
     <sheet name="Test Suite" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>TSID</t>
   </si>
@@ -28,9 +28,6 @@
     <t>Login functionality</t>
   </si>
   <si>
-    <t>Check out</t>
-  </si>
-  <si>
     <t>My Account</t>
   </si>
   <si>
@@ -38,12 +35,6 @@
   </si>
   <si>
     <t>Account details</t>
-  </si>
-  <si>
-    <t>CheckoutScenarios</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
   <si>
     <t>Y</t>
@@ -129,19 +120,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -447,21 +432,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="23.26953125" style="2" customWidth="1"/>
     <col min="2" max="2" width="35" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="2"/>
+    <col min="3" max="3" width="9.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -472,37 +457,26 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pushign the changes done for runmodes -4 TC
</commit_message>
<xml_diff>
--- a/src/test/java/com/born/xls/Suite.xlsx
+++ b/src/test/java/com/born/xls/Suite.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>TSID</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -435,7 +438,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -465,7 +468,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>